<commit_message>
Updated diary - thuc nguyen
</commit_message>
<xml_diff>
--- a/diaries/diary-thuc-nguyen.xlsx
+++ b/diaries/diary-thuc-nguyen.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -153,6 +153,70 @@
     <t>The articles were interesting and provided more perspectives on how to read code. Something that I was found interesting and must remind myself to stress is hidden state machines because I used to get by with flags.  I felt like this activity helped tie together what we learned in class about reading code.</t>
   </si>
   <si>
+    <t>I wanted to underestand what mental models were and what and how to use a UML diagram.</t>
+  </si>
+  <si>
+    <t>1) Understood what mental models are and how we use them
+2) What UML diagrams are, its usages, and how they can help look at the architecture of the code, its relationships, and its flow</t>
+  </si>
+  <si>
+    <t>I learned that we use mental models as a way to represent how we perceive things to work in the real world. The importance of mental models is evident for users who act upon a system based on what they understand about past software they have used. Menal models also affect developers because they should also consider other developers' mental models when forming their software system. I learned that mental models have limitations as well. 
+In regards to UML diagrams, they are visualized with boxes as classes or interfaces, in which each box contains variables, getters, and setters. The lines portray the relationships of each class to one another.</t>
+  </si>
+  <si>
+    <t>The activity gave me more information on what people use to read and understand code, with mental models and UML diagrams being examples. The mood was enlightening.</t>
+  </si>
+  <si>
+    <t>Readings - Reading code (diagrams and mental models)</t>
+  </si>
+  <si>
+    <t>1) Ways in which people externalize their mental models and visualize representations of how they read code
+2) Useful techniques to help externalize</t>
+  </si>
+  <si>
+    <t>I learned that one way to read code is to write out, in acronyms even, the constructors and/or methods of a class in a simplistic form to see what it roughly does. Strategies for working with legacy code include trying to create a mapping or a data model and to beware for and find bugs to fix. Try to communicate with any stakeholders but also future developers that will look at your code by providing better documentation or writing down the representation of the system. Keep a log, keep in mind business needs, and leave the code in better shape.</t>
+  </si>
+  <si>
+    <t>The activity was okay. It elaborated more on last week's readings.</t>
+  </si>
+  <si>
+    <t>3:00pm - 5:00pm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project
+Printing out a UML diagram of the project
+</t>
+  </si>
+  <si>
+    <t>1) Was able to print out the UML diagram, which was around 20 pages. I loaded the UML on the entire runelite folder, and although it loaded properly, Deon suggested loading only the UML diagram for the client package since that's our primary focus.</t>
+  </si>
+  <si>
+    <t>It was, according to Deon, tough to print out the diagram in png, because it was overall about 60mb of memory, and this was compressed. It took a lot of ram for him to load the image on gimp, which would be impossible on my own laptop.</t>
+  </si>
+  <si>
+    <t>Activity was tough because without Deon's help and his access to a pretty strong computer, with a lot of ram, we would probably have had a harder time than we did.</t>
+  </si>
+  <si>
+    <t>9:00pm - 11:00pm</t>
+  </si>
+  <si>
+    <t>Project
+- Highlight 2 features in diagram where they are implemented
+- Use templates
+- Complete a writeup</t>
+  </si>
+  <si>
+    <t>1) Highlighted the 2 features in the diagram
+2) Used the templates to help us navigate through the code
+3) Completed the writeup</t>
+  </si>
+  <si>
+    <t>We had to use the UML diagram generated on IntelliJ first to help us find where the classes are before highlighting it on the printed diagram. The 2 features we chose were the ScreenMarker feature of the client which allowed players to mark on the screen boxes of a customizable color to help them mark the exact positions of things. The other feature was the metronome feature which was a supporting timing feature. We used the templates to write down where we've been in the code and where to go, and although it was very tedious, it helped us navigate through the files under the screenmarker and metronome plugin packages. We were able to understand more about what the code did which helped us write more detailed information on the writeup.</t>
+  </si>
+  <si>
+    <t>Overall, the activity was a bit exhausting with the use of the templates, but I understand how it can be helpful, since we are thinking at every step, and making decisions on where to go from where we are.</t>
+  </si>
+  <si>
     <t>&lt;what day?&gt;</t>
   </si>
   <si>
@@ -178,12 +242,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="166" formatCode="h:mm am/pm"/>
+    <numFmt numFmtId="167" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -200,15 +265,18 @@
       <b/>
       <sz val="12.0"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <i/>
       <sz val="12.0"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11.0"/>
       <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <i/>
@@ -220,6 +288,23 @@
       <b/>
       <sz val="12.0"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12.0"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11.0"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <i/>
@@ -230,10 +315,6 @@
       <i/>
       <sz val="11.0"/>
       <color rgb="FF006100"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="5">
@@ -285,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -321,7 +402,7 @@
     <xf borderId="4" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf borderId="4" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -342,8 +423,23 @@
     <xf borderId="4" fillId="4" fontId="8" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="top"/>
+    <xf borderId="4" fillId="4" fontId="11" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="11" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="11" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -723,11 +819,11 @@
       <c r="G8" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="18">
@@ -775,216 +871,212 @@
       <c r="G10" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
     </row>
     <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="20">
+        <v>43853.0</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="E11" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="F11" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="G11" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+    </row>
+    <row r="12" ht="14.25" customHeight="1">
+      <c r="A12" s="20">
+        <v>43857.0</v>
+      </c>
+      <c r="B12" s="24">
+        <v>0.8541666666666666</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="E12" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="F12" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="20"/>
-    </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="15" t="s">
-        <v>36</v>
+      <c r="G12" s="23" t="s">
+        <v>43</v>
       </c>
-      <c r="B12" s="15" t="s">
-        <v>37</v>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+    </row>
+    <row r="13" ht="14.25" customHeight="1">
+      <c r="A13" s="20">
+        <v>43859.0</v>
       </c>
-      <c r="C12" s="15" t="s">
-        <v>38</v>
+      <c r="B13" s="21" t="s">
+        <v>44</v>
       </c>
-      <c r="D12" s="15" t="s">
-        <v>39</v>
+      <c r="C13" s="21" t="s">
+        <v>23</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>40</v>
+      <c r="D13" s="21" t="s">
+        <v>45</v>
       </c>
-      <c r="F12" s="15" t="s">
-        <v>41</v>
+      <c r="E13" s="21" t="s">
+        <v>46</v>
       </c>
-      <c r="G12" s="21" t="s">
-        <v>42</v>
+      <c r="F13" s="21" t="s">
+        <v>47</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
-    </row>
-    <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="15" t="s">
-        <v>36</v>
+      <c r="G13" s="23" t="s">
+        <v>48</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>37</v>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+    </row>
+    <row r="14" ht="14.25" customHeight="1">
+      <c r="A14" s="25">
+        <v>43859.0</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>38</v>
+      <c r="B14" s="21" t="s">
+        <v>49</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>39</v>
+      <c r="C14" s="21" t="s">
+        <v>23</v>
       </c>
-      <c r="E13" s="15" t="s">
-        <v>40</v>
+      <c r="D14" s="21" t="s">
+        <v>50</v>
       </c>
-      <c r="F13" s="15" t="s">
-        <v>41</v>
+      <c r="E14" s="21" t="s">
+        <v>51</v>
       </c>
-      <c r="G13" s="21" t="s">
-        <v>42</v>
+      <c r="F14" s="21" t="s">
+        <v>52</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-    </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="15" t="s">
-        <v>36</v>
+      <c r="G14" s="23" t="s">
+        <v>53</v>
       </c>
-      <c r="B14" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="20"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
-      <c r="G15" s="21" t="s">
-        <v>42</v>
+      <c r="G15" s="26" t="s">
+        <v>60</v>
       </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="A16" s="15" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
-      <c r="G16" s="21" t="s">
-        <v>42</v>
+      <c r="G16" s="26" t="s">
+        <v>60</v>
       </c>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
     </row>
     <row r="17" ht="14.25" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
-      <c r="G17" s="21" t="s">
-        <v>42</v>
+      <c r="G17" s="26" t="s">
+        <v>60</v>
       </c>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
       <c r="A18" s="15"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
-      <c r="D18" s="21"/>
+      <c r="D18" s="26"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
-      <c r="G18" s="21"/>
+      <c r="G18" s="26"/>
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
       <c r="J18" s="17"/>
@@ -998,7 +1090,7 @@
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
-      <c r="G19" s="21"/>
+      <c r="G19" s="26"/>
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
@@ -1012,7 +1104,7 @@
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="21"/>
+      <c r="G20" s="26"/>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
       <c r="J20" s="17"/>
@@ -1026,7 +1118,7 @@
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
-      <c r="G21" s="21"/>
+      <c r="G21" s="26"/>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>
       <c r="J21" s="17"/>
@@ -1040,7 +1132,7 @@
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
-      <c r="G22" s="21"/>
+      <c r="G22" s="26"/>
       <c r="H22" s="17"/>
       <c r="I22" s="17"/>
       <c r="J22" s="17"/>
@@ -1054,7 +1146,7 @@
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
-      <c r="G23" s="21"/>
+      <c r="G23" s="26"/>
       <c r="H23" s="17"/>
       <c r="I23" s="17"/>
       <c r="J23" s="17"/>
@@ -1068,7 +1160,7 @@
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
-      <c r="G24" s="21"/>
+      <c r="G24" s="26"/>
       <c r="H24" s="17"/>
       <c r="I24" s="17"/>
       <c r="J24" s="17"/>
@@ -1082,7 +1174,7 @@
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
       <c r="F25" s="15"/>
-      <c r="G25" s="21"/>
+      <c r="G25" s="26"/>
       <c r="H25" s="17"/>
       <c r="I25" s="17"/>
       <c r="J25" s="17"/>
@@ -1096,7 +1188,7 @@
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
-      <c r="G26" s="21"/>
+      <c r="G26" s="26"/>
       <c r="H26" s="17"/>
       <c r="I26" s="17"/>
       <c r="J26" s="17"/>
@@ -1110,7 +1202,7 @@
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
-      <c r="G27" s="21"/>
+      <c r="G27" s="26"/>
       <c r="H27" s="17"/>
       <c r="I27" s="17"/>
       <c r="J27" s="17"/>
@@ -1124,7 +1216,7 @@
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
-      <c r="G28" s="21"/>
+      <c r="G28" s="26"/>
       <c r="H28" s="17"/>
       <c r="I28" s="17"/>
       <c r="J28" s="17"/>
@@ -1138,7 +1230,7 @@
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
-      <c r="G29" s="21"/>
+      <c r="G29" s="26"/>
       <c r="H29" s="17"/>
       <c r="I29" s="17"/>
       <c r="J29" s="17"/>
@@ -1152,7 +1244,7 @@
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
-      <c r="G30" s="21"/>
+      <c r="G30" s="26"/>
       <c r="H30" s="17"/>
       <c r="I30" s="17"/>
       <c r="J30" s="17"/>
@@ -1166,7 +1258,7 @@
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
       <c r="F31" s="15"/>
-      <c r="G31" s="21"/>
+      <c r="G31" s="26"/>
       <c r="H31" s="17"/>
       <c r="I31" s="17"/>
       <c r="J31" s="17"/>
@@ -1180,7 +1272,7 @@
       <c r="D32" s="15"/>
       <c r="E32" s="15"/>
       <c r="F32" s="15"/>
-      <c r="G32" s="21"/>
+      <c r="G32" s="26"/>
       <c r="H32" s="17"/>
       <c r="I32" s="17"/>
       <c r="J32" s="17"/>
@@ -1194,7 +1286,7 @@
       <c r="D33" s="15"/>
       <c r="E33" s="15"/>
       <c r="F33" s="15"/>
-      <c r="G33" s="21"/>
+      <c r="G33" s="26"/>
       <c r="H33" s="17"/>
       <c r="I33" s="17"/>
       <c r="J33" s="17"/>
@@ -1208,7 +1300,7 @@
       <c r="D34" s="15"/>
       <c r="E34" s="15"/>
       <c r="F34" s="15"/>
-      <c r="G34" s="21"/>
+      <c r="G34" s="26"/>
       <c r="H34" s="17"/>
       <c r="I34" s="17"/>
       <c r="J34" s="17"/>
@@ -1222,7 +1314,7 @@
       <c r="D35" s="15"/>
       <c r="E35" s="15"/>
       <c r="F35" s="15"/>
-      <c r="G35" s="21"/>
+      <c r="G35" s="26"/>
       <c r="H35" s="17"/>
       <c r="I35" s="17"/>
       <c r="J35" s="17"/>
@@ -1236,7 +1328,7 @@
       <c r="D36" s="15"/>
       <c r="E36" s="15"/>
       <c r="F36" s="15"/>
-      <c r="G36" s="21"/>
+      <c r="G36" s="26"/>
       <c r="H36" s="17"/>
       <c r="I36" s="17"/>
       <c r="J36" s="17"/>
@@ -1250,7 +1342,7 @@
       <c r="D37" s="15"/>
       <c r="E37" s="15"/>
       <c r="F37" s="15"/>
-      <c r="G37" s="21"/>
+      <c r="G37" s="26"/>
       <c r="H37" s="17"/>
       <c r="I37" s="17"/>
       <c r="J37" s="17"/>
@@ -1264,7 +1356,7 @@
       <c r="D38" s="15"/>
       <c r="E38" s="15"/>
       <c r="F38" s="15"/>
-      <c r="G38" s="21"/>
+      <c r="G38" s="26"/>
       <c r="H38" s="17"/>
       <c r="I38" s="17"/>
       <c r="J38" s="17"/>
@@ -1278,7 +1370,7 @@
       <c r="D39" s="15"/>
       <c r="E39" s="15"/>
       <c r="F39" s="15"/>
-      <c r="G39" s="21"/>
+      <c r="G39" s="26"/>
       <c r="H39" s="17"/>
       <c r="I39" s="17"/>
       <c r="J39" s="17"/>
@@ -1292,7 +1384,7 @@
       <c r="D40" s="15"/>
       <c r="E40" s="15"/>
       <c r="F40" s="15"/>
-      <c r="G40" s="21"/>
+      <c r="G40" s="26"/>
       <c r="H40" s="17"/>
       <c r="I40" s="17"/>
       <c r="J40" s="17"/>
@@ -1306,7 +1398,7 @@
       <c r="D41" s="15"/>
       <c r="E41" s="15"/>
       <c r="F41" s="15"/>
-      <c r="G41" s="21"/>
+      <c r="G41" s="26"/>
       <c r="H41" s="17"/>
       <c r="I41" s="17"/>
       <c r="J41" s="17"/>
@@ -1320,7 +1412,7 @@
       <c r="D42" s="15"/>
       <c r="E42" s="15"/>
       <c r="F42" s="15"/>
-      <c r="G42" s="21"/>
+      <c r="G42" s="26"/>
       <c r="H42" s="17"/>
       <c r="I42" s="17"/>
       <c r="J42" s="17"/>
@@ -1334,7 +1426,7 @@
       <c r="D43" s="15"/>
       <c r="E43" s="15"/>
       <c r="F43" s="15"/>
-      <c r="G43" s="21"/>
+      <c r="G43" s="26"/>
       <c r="H43" s="17"/>
       <c r="I43" s="17"/>
       <c r="J43" s="17"/>
@@ -1348,7 +1440,7 @@
       <c r="D44" s="15"/>
       <c r="E44" s="15"/>
       <c r="F44" s="15"/>
-      <c r="G44" s="21"/>
+      <c r="G44" s="26"/>
       <c r="H44" s="17"/>
       <c r="I44" s="17"/>
       <c r="J44" s="17"/>
@@ -1362,7 +1454,7 @@
       <c r="D45" s="15"/>
       <c r="E45" s="15"/>
       <c r="F45" s="15"/>
-      <c r="G45" s="21"/>
+      <c r="G45" s="26"/>
       <c r="H45" s="17"/>
       <c r="I45" s="17"/>
       <c r="J45" s="17"/>
@@ -1376,7 +1468,7 @@
       <c r="D46" s="15"/>
       <c r="E46" s="15"/>
       <c r="F46" s="15"/>
-      <c r="G46" s="21"/>
+      <c r="G46" s="26"/>
       <c r="H46" s="17"/>
       <c r="I46" s="17"/>
       <c r="J46" s="17"/>
@@ -1390,7 +1482,7 @@
       <c r="D47" s="15"/>
       <c r="E47" s="15"/>
       <c r="F47" s="15"/>
-      <c r="G47" s="21"/>
+      <c r="G47" s="26"/>
       <c r="H47" s="17"/>
       <c r="I47" s="17"/>
       <c r="J47" s="17"/>
@@ -1404,7 +1496,7 @@
       <c r="D48" s="15"/>
       <c r="E48" s="15"/>
       <c r="F48" s="15"/>
-      <c r="G48" s="21"/>
+      <c r="G48" s="26"/>
       <c r="H48" s="17"/>
       <c r="I48" s="17"/>
       <c r="J48" s="17"/>
@@ -1418,7 +1510,7 @@
       <c r="D49" s="15"/>
       <c r="E49" s="15"/>
       <c r="F49" s="15"/>
-      <c r="G49" s="21"/>
+      <c r="G49" s="26"/>
       <c r="H49" s="17"/>
       <c r="I49" s="17"/>
       <c r="J49" s="17"/>
@@ -1432,7 +1524,7 @@
       <c r="D50" s="15"/>
       <c r="E50" s="15"/>
       <c r="F50" s="15"/>
-      <c r="G50" s="21"/>
+      <c r="G50" s="26"/>
       <c r="H50" s="17"/>
       <c r="I50" s="17"/>
       <c r="J50" s="17"/>
@@ -1446,7 +1538,7 @@
       <c r="D51" s="15"/>
       <c r="E51" s="15"/>
       <c r="F51" s="15"/>
-      <c r="G51" s="21"/>
+      <c r="G51" s="26"/>
       <c r="H51" s="17"/>
       <c r="I51" s="17"/>
       <c r="J51" s="17"/>
@@ -1460,7 +1552,7 @@
       <c r="D52" s="15"/>
       <c r="E52" s="15"/>
       <c r="F52" s="15"/>
-      <c r="G52" s="21"/>
+      <c r="G52" s="26"/>
       <c r="H52" s="17"/>
       <c r="I52" s="17"/>
       <c r="J52" s="17"/>
@@ -1474,7 +1566,7 @@
       <c r="D53" s="15"/>
       <c r="E53" s="15"/>
       <c r="F53" s="15"/>
-      <c r="G53" s="21"/>
+      <c r="G53" s="26"/>
       <c r="H53" s="17"/>
       <c r="I53" s="17"/>
       <c r="J53" s="17"/>
@@ -1488,7 +1580,7 @@
       <c r="D54" s="15"/>
       <c r="E54" s="15"/>
       <c r="F54" s="15"/>
-      <c r="G54" s="21"/>
+      <c r="G54" s="26"/>
       <c r="H54" s="17"/>
       <c r="I54" s="17"/>
       <c r="J54" s="17"/>
@@ -1502,7 +1594,7 @@
       <c r="D55" s="15"/>
       <c r="E55" s="15"/>
       <c r="F55" s="15"/>
-      <c r="G55" s="21"/>
+      <c r="G55" s="26"/>
       <c r="H55" s="17"/>
       <c r="I55" s="17"/>
       <c r="J55" s="17"/>
@@ -1516,7 +1608,7 @@
       <c r="D56" s="15"/>
       <c r="E56" s="15"/>
       <c r="F56" s="15"/>
-      <c r="G56" s="21"/>
+      <c r="G56" s="26"/>
       <c r="H56" s="17"/>
       <c r="I56" s="17"/>
       <c r="J56" s="17"/>
@@ -1530,7 +1622,7 @@
       <c r="D57" s="15"/>
       <c r="E57" s="15"/>
       <c r="F57" s="15"/>
-      <c r="G57" s="21"/>
+      <c r="G57" s="26"/>
       <c r="H57" s="17"/>
       <c r="I57" s="17"/>
       <c r="J57" s="17"/>
@@ -1544,7 +1636,7 @@
       <c r="D58" s="15"/>
       <c r="E58" s="15"/>
       <c r="F58" s="15"/>
-      <c r="G58" s="21"/>
+      <c r="G58" s="26"/>
       <c r="H58" s="17"/>
       <c r="I58" s="17"/>
       <c r="J58" s="17"/>
@@ -1558,7 +1650,7 @@
       <c r="D59" s="15"/>
       <c r="E59" s="15"/>
       <c r="F59" s="15"/>
-      <c r="G59" s="21"/>
+      <c r="G59" s="26"/>
       <c r="H59" s="17"/>
       <c r="I59" s="17"/>
       <c r="J59" s="17"/>
@@ -1572,7 +1664,7 @@
       <c r="D60" s="15"/>
       <c r="E60" s="15"/>
       <c r="F60" s="15"/>
-      <c r="G60" s="21"/>
+      <c r="G60" s="26"/>
       <c r="H60" s="17"/>
       <c r="I60" s="17"/>
       <c r="J60" s="17"/>
@@ -1586,7 +1678,7 @@
       <c r="D61" s="15"/>
       <c r="E61" s="15"/>
       <c r="F61" s="15"/>
-      <c r="G61" s="21"/>
+      <c r="G61" s="26"/>
       <c r="H61" s="17"/>
       <c r="I61" s="17"/>
       <c r="J61" s="17"/>
@@ -1600,7 +1692,7 @@
       <c r="D62" s="15"/>
       <c r="E62" s="15"/>
       <c r="F62" s="15"/>
-      <c r="G62" s="21"/>
+      <c r="G62" s="26"/>
       <c r="H62" s="17"/>
       <c r="I62" s="17"/>
       <c r="J62" s="17"/>
@@ -1614,7 +1706,7 @@
       <c r="D63" s="15"/>
       <c r="E63" s="15"/>
       <c r="F63" s="15"/>
-      <c r="G63" s="21"/>
+      <c r="G63" s="26"/>
       <c r="H63" s="17"/>
       <c r="I63" s="17"/>
       <c r="J63" s="17"/>
@@ -1628,7 +1720,7 @@
       <c r="D64" s="15"/>
       <c r="E64" s="15"/>
       <c r="F64" s="15"/>
-      <c r="G64" s="21"/>
+      <c r="G64" s="26"/>
       <c r="H64" s="17"/>
       <c r="I64" s="17"/>
       <c r="J64" s="17"/>
@@ -1642,7 +1734,7 @@
       <c r="D65" s="15"/>
       <c r="E65" s="15"/>
       <c r="F65" s="15"/>
-      <c r="G65" s="21"/>
+      <c r="G65" s="26"/>
       <c r="H65" s="17"/>
       <c r="I65" s="17"/>
       <c r="J65" s="17"/>
@@ -1656,7 +1748,7 @@
       <c r="D66" s="15"/>
       <c r="E66" s="15"/>
       <c r="F66" s="15"/>
-      <c r="G66" s="21"/>
+      <c r="G66" s="26"/>
       <c r="H66" s="17"/>
       <c r="I66" s="17"/>
       <c r="J66" s="17"/>
@@ -1670,7 +1762,7 @@
       <c r="D67" s="15"/>
       <c r="E67" s="15"/>
       <c r="F67" s="15"/>
-      <c r="G67" s="21"/>
+      <c r="G67" s="26"/>
       <c r="H67" s="17"/>
       <c r="I67" s="17"/>
       <c r="J67" s="17"/>
@@ -1684,7 +1776,7 @@
       <c r="D68" s="15"/>
       <c r="E68" s="15"/>
       <c r="F68" s="15"/>
-      <c r="G68" s="21"/>
+      <c r="G68" s="26"/>
       <c r="H68" s="17"/>
       <c r="I68" s="17"/>
       <c r="J68" s="17"/>
@@ -1698,7 +1790,7 @@
       <c r="D69" s="15"/>
       <c r="E69" s="15"/>
       <c r="F69" s="15"/>
-      <c r="G69" s="21"/>
+      <c r="G69" s="26"/>
       <c r="H69" s="17"/>
       <c r="I69" s="17"/>
       <c r="J69" s="17"/>
@@ -1712,7 +1804,7 @@
       <c r="D70" s="15"/>
       <c r="E70" s="15"/>
       <c r="F70" s="15"/>
-      <c r="G70" s="21"/>
+      <c r="G70" s="26"/>
       <c r="H70" s="17"/>
       <c r="I70" s="17"/>
       <c r="J70" s="17"/>
@@ -1726,7 +1818,7 @@
       <c r="D71" s="15"/>
       <c r="E71" s="15"/>
       <c r="F71" s="15"/>
-      <c r="G71" s="21"/>
+      <c r="G71" s="26"/>
       <c r="H71" s="17"/>
       <c r="I71" s="17"/>
       <c r="J71" s="17"/>
@@ -1740,7 +1832,7 @@
       <c r="D72" s="15"/>
       <c r="E72" s="15"/>
       <c r="F72" s="15"/>
-      <c r="G72" s="21"/>
+      <c r="G72" s="26"/>
       <c r="H72" s="17"/>
       <c r="I72" s="17"/>
       <c r="J72" s="17"/>
@@ -1754,7 +1846,7 @@
       <c r="D73" s="15"/>
       <c r="E73" s="15"/>
       <c r="F73" s="15"/>
-      <c r="G73" s="21"/>
+      <c r="G73" s="26"/>
       <c r="H73" s="17"/>
       <c r="I73" s="17"/>
       <c r="J73" s="17"/>
@@ -1768,7 +1860,7 @@
       <c r="D74" s="15"/>
       <c r="E74" s="15"/>
       <c r="F74" s="15"/>
-      <c r="G74" s="21"/>
+      <c r="G74" s="26"/>
       <c r="H74" s="17"/>
       <c r="I74" s="17"/>
       <c r="J74" s="17"/>
@@ -1782,7 +1874,7 @@
       <c r="D75" s="15"/>
       <c r="E75" s="15"/>
       <c r="F75" s="15"/>
-      <c r="G75" s="21"/>
+      <c r="G75" s="26"/>
       <c r="H75" s="17"/>
       <c r="I75" s="17"/>
       <c r="J75" s="17"/>
@@ -1796,7 +1888,7 @@
       <c r="D76" s="15"/>
       <c r="E76" s="15"/>
       <c r="F76" s="15"/>
-      <c r="G76" s="21"/>
+      <c r="G76" s="26"/>
       <c r="H76" s="17"/>
       <c r="I76" s="17"/>
       <c r="J76" s="17"/>
@@ -1810,7 +1902,7 @@
       <c r="D77" s="15"/>
       <c r="E77" s="15"/>
       <c r="F77" s="15"/>
-      <c r="G77" s="21"/>
+      <c r="G77" s="26"/>
       <c r="H77" s="17"/>
       <c r="I77" s="17"/>
       <c r="J77" s="17"/>
@@ -1824,7 +1916,7 @@
       <c r="D78" s="15"/>
       <c r="E78" s="15"/>
       <c r="F78" s="15"/>
-      <c r="G78" s="21"/>
+      <c r="G78" s="26"/>
       <c r="H78" s="17"/>
       <c r="I78" s="17"/>
       <c r="J78" s="17"/>
@@ -1838,7 +1930,7 @@
       <c r="D79" s="15"/>
       <c r="E79" s="15"/>
       <c r="F79" s="15"/>
-      <c r="G79" s="21"/>
+      <c r="G79" s="26"/>
       <c r="H79" s="17"/>
       <c r="I79" s="17"/>
       <c r="J79" s="17"/>
@@ -1852,7 +1944,7 @@
       <c r="D80" s="15"/>
       <c r="E80" s="15"/>
       <c r="F80" s="15"/>
-      <c r="G80" s="21"/>
+      <c r="G80" s="26"/>
       <c r="H80" s="17"/>
       <c r="I80" s="17"/>
       <c r="J80" s="17"/>
@@ -1866,7 +1958,7 @@
       <c r="D81" s="15"/>
       <c r="E81" s="15"/>
       <c r="F81" s="15"/>
-      <c r="G81" s="21"/>
+      <c r="G81" s="26"/>
       <c r="H81" s="17"/>
       <c r="I81" s="17"/>
       <c r="J81" s="17"/>
@@ -1880,7 +1972,7 @@
       <c r="D82" s="15"/>
       <c r="E82" s="15"/>
       <c r="F82" s="15"/>
-      <c r="G82" s="21"/>
+      <c r="G82" s="26"/>
       <c r="H82" s="17"/>
       <c r="I82" s="17"/>
       <c r="J82" s="17"/>
@@ -1894,7 +1986,7 @@
       <c r="D83" s="15"/>
       <c r="E83" s="15"/>
       <c r="F83" s="15"/>
-      <c r="G83" s="21"/>
+      <c r="G83" s="26"/>
       <c r="H83" s="17"/>
       <c r="I83" s="17"/>
       <c r="J83" s="17"/>
@@ -1908,7 +2000,7 @@
       <c r="D84" s="15"/>
       <c r="E84" s="15"/>
       <c r="F84" s="15"/>
-      <c r="G84" s="21"/>
+      <c r="G84" s="26"/>
       <c r="H84" s="17"/>
       <c r="I84" s="17"/>
       <c r="J84" s="17"/>
@@ -1922,7 +2014,7 @@
       <c r="D85" s="15"/>
       <c r="E85" s="15"/>
       <c r="F85" s="15"/>
-      <c r="G85" s="21"/>
+      <c r="G85" s="26"/>
       <c r="H85" s="17"/>
       <c r="I85" s="17"/>
       <c r="J85" s="17"/>
@@ -1936,7 +2028,7 @@
       <c r="D86" s="15"/>
       <c r="E86" s="15"/>
       <c r="F86" s="15"/>
-      <c r="G86" s="21"/>
+      <c r="G86" s="26"/>
       <c r="H86" s="17"/>
       <c r="I86" s="17"/>
       <c r="J86" s="17"/>
@@ -1950,7 +2042,7 @@
       <c r="D87" s="15"/>
       <c r="E87" s="15"/>
       <c r="F87" s="15"/>
-      <c r="G87" s="21"/>
+      <c r="G87" s="26"/>
       <c r="H87" s="17"/>
       <c r="I87" s="17"/>
       <c r="J87" s="17"/>
@@ -1964,7 +2056,7 @@
       <c r="D88" s="15"/>
       <c r="E88" s="15"/>
       <c r="F88" s="15"/>
-      <c r="G88" s="21"/>
+      <c r="G88" s="26"/>
       <c r="H88" s="17"/>
       <c r="I88" s="17"/>
       <c r="J88" s="17"/>
@@ -1978,7 +2070,7 @@
       <c r="D89" s="15"/>
       <c r="E89" s="15"/>
       <c r="F89" s="15"/>
-      <c r="G89" s="21"/>
+      <c r="G89" s="26"/>
       <c r="H89" s="17"/>
       <c r="I89" s="17"/>
       <c r="J89" s="17"/>
@@ -1992,7 +2084,7 @@
       <c r="D90" s="15"/>
       <c r="E90" s="15"/>
       <c r="F90" s="15"/>
-      <c r="G90" s="21"/>
+      <c r="G90" s="26"/>
       <c r="H90" s="17"/>
       <c r="I90" s="17"/>
       <c r="J90" s="17"/>
@@ -2006,7 +2098,7 @@
       <c r="D91" s="15"/>
       <c r="E91" s="15"/>
       <c r="F91" s="15"/>
-      <c r="G91" s="21"/>
+      <c r="G91" s="26"/>
       <c r="H91" s="17"/>
       <c r="I91" s="17"/>
       <c r="J91" s="17"/>
@@ -2020,7 +2112,7 @@
       <c r="D92" s="15"/>
       <c r="E92" s="15"/>
       <c r="F92" s="15"/>
-      <c r="G92" s="21"/>
+      <c r="G92" s="26"/>
       <c r="H92" s="17"/>
       <c r="I92" s="17"/>
       <c r="J92" s="17"/>
@@ -2034,7 +2126,7 @@
       <c r="D93" s="15"/>
       <c r="E93" s="15"/>
       <c r="F93" s="15"/>
-      <c r="G93" s="21"/>
+      <c r="G93" s="26"/>
       <c r="H93" s="17"/>
       <c r="I93" s="17"/>
       <c r="J93" s="17"/>
@@ -2048,7 +2140,7 @@
       <c r="D94" s="15"/>
       <c r="E94" s="15"/>
       <c r="F94" s="15"/>
-      <c r="G94" s="21"/>
+      <c r="G94" s="26"/>
       <c r="H94" s="17"/>
       <c r="I94" s="17"/>
       <c r="J94" s="17"/>
@@ -2062,7 +2154,7 @@
       <c r="D95" s="15"/>
       <c r="E95" s="15"/>
       <c r="F95" s="15"/>
-      <c r="G95" s="21"/>
+      <c r="G95" s="26"/>
       <c r="H95" s="17"/>
       <c r="I95" s="17"/>
       <c r="J95" s="17"/>
@@ -2076,7 +2168,7 @@
       <c r="D96" s="15"/>
       <c r="E96" s="15"/>
       <c r="F96" s="15"/>
-      <c r="G96" s="21"/>
+      <c r="G96" s="26"/>
       <c r="H96" s="17"/>
       <c r="I96" s="17"/>
       <c r="J96" s="17"/>
@@ -2090,7 +2182,7 @@
       <c r="D97" s="15"/>
       <c r="E97" s="15"/>
       <c r="F97" s="15"/>
-      <c r="G97" s="21"/>
+      <c r="G97" s="26"/>
       <c r="H97" s="17"/>
       <c r="I97" s="17"/>
       <c r="J97" s="17"/>
@@ -2104,7 +2196,7 @@
       <c r="D98" s="15"/>
       <c r="E98" s="15"/>
       <c r="F98" s="15"/>
-      <c r="G98" s="21"/>
+      <c r="G98" s="26"/>
       <c r="H98" s="17"/>
       <c r="I98" s="17"/>
       <c r="J98" s="17"/>
@@ -2118,7 +2210,7 @@
       <c r="D99" s="15"/>
       <c r="E99" s="15"/>
       <c r="F99" s="15"/>
-      <c r="G99" s="21"/>
+      <c r="G99" s="26"/>
       <c r="H99" s="17"/>
       <c r="I99" s="17"/>
       <c r="J99" s="17"/>
@@ -2132,7 +2224,7 @@
       <c r="D100" s="15"/>
       <c r="E100" s="15"/>
       <c r="F100" s="15"/>
-      <c r="G100" s="21"/>
+      <c r="G100" s="26"/>
       <c r="H100" s="17"/>
       <c r="I100" s="17"/>
       <c r="J100" s="17"/>
@@ -2146,7 +2238,7 @@
       <c r="D101" s="15"/>
       <c r="E101" s="15"/>
       <c r="F101" s="15"/>
-      <c r="G101" s="21"/>
+      <c r="G101" s="26"/>
       <c r="H101" s="17"/>
       <c r="I101" s="17"/>
       <c r="J101" s="17"/>
@@ -2160,7 +2252,7 @@
       <c r="D102" s="15"/>
       <c r="E102" s="15"/>
       <c r="F102" s="15"/>
-      <c r="G102" s="21"/>
+      <c r="G102" s="26"/>
       <c r="H102" s="17"/>
       <c r="I102" s="17"/>
       <c r="J102" s="17"/>
@@ -2174,7 +2266,7 @@
       <c r="D103" s="15"/>
       <c r="E103" s="15"/>
       <c r="F103" s="15"/>
-      <c r="G103" s="21"/>
+      <c r="G103" s="26"/>
       <c r="H103" s="17"/>
       <c r="I103" s="17"/>
       <c r="J103" s="17"/>
@@ -2188,7 +2280,7 @@
       <c r="D104" s="15"/>
       <c r="E104" s="15"/>
       <c r="F104" s="15"/>
-      <c r="G104" s="21"/>
+      <c r="G104" s="26"/>
       <c r="H104" s="17"/>
       <c r="I104" s="17"/>
       <c r="J104" s="17"/>
@@ -2202,7 +2294,7 @@
       <c r="D105" s="15"/>
       <c r="E105" s="15"/>
       <c r="F105" s="15"/>
-      <c r="G105" s="21"/>
+      <c r="G105" s="26"/>
       <c r="H105" s="17"/>
       <c r="I105" s="17"/>
       <c r="J105" s="17"/>
@@ -2216,7 +2308,7 @@
       <c r="D106" s="15"/>
       <c r="E106" s="15"/>
       <c r="F106" s="15"/>
-      <c r="G106" s="21"/>
+      <c r="G106" s="26"/>
       <c r="H106" s="17"/>
       <c r="I106" s="17"/>
       <c r="J106" s="17"/>
@@ -2230,7 +2322,7 @@
       <c r="D107" s="15"/>
       <c r="E107" s="15"/>
       <c r="F107" s="15"/>
-      <c r="G107" s="21"/>
+      <c r="G107" s="26"/>
       <c r="H107" s="17"/>
       <c r="I107" s="17"/>
       <c r="J107" s="17"/>
@@ -2244,7 +2336,7 @@
       <c r="D108" s="15"/>
       <c r="E108" s="15"/>
       <c r="F108" s="15"/>
-      <c r="G108" s="21"/>
+      <c r="G108" s="26"/>
       <c r="H108" s="17"/>
       <c r="I108" s="17"/>
       <c r="J108" s="17"/>
@@ -2258,7 +2350,7 @@
       <c r="D109" s="15"/>
       <c r="E109" s="15"/>
       <c r="F109" s="15"/>
-      <c r="G109" s="21"/>
+      <c r="G109" s="26"/>
       <c r="H109" s="17"/>
       <c r="I109" s="17"/>
       <c r="J109" s="17"/>
@@ -2272,7 +2364,7 @@
       <c r="D110" s="15"/>
       <c r="E110" s="15"/>
       <c r="F110" s="15"/>
-      <c r="G110" s="21"/>
+      <c r="G110" s="26"/>
       <c r="H110" s="17"/>
       <c r="I110" s="17"/>
       <c r="J110" s="17"/>
@@ -2286,7 +2378,7 @@
       <c r="D111" s="15"/>
       <c r="E111" s="15"/>
       <c r="F111" s="15"/>
-      <c r="G111" s="21"/>
+      <c r="G111" s="26"/>
       <c r="H111" s="17"/>
       <c r="I111" s="17"/>
       <c r="J111" s="17"/>
@@ -2300,7 +2392,7 @@
       <c r="D112" s="15"/>
       <c r="E112" s="15"/>
       <c r="F112" s="15"/>
-      <c r="G112" s="21"/>
+      <c r="G112" s="26"/>
       <c r="H112" s="17"/>
       <c r="I112" s="17"/>
       <c r="J112" s="17"/>
@@ -2314,7 +2406,7 @@
       <c r="D113" s="15"/>
       <c r="E113" s="15"/>
       <c r="F113" s="15"/>
-      <c r="G113" s="21"/>
+      <c r="G113" s="26"/>
       <c r="H113" s="17"/>
       <c r="I113" s="17"/>
       <c r="J113" s="17"/>
@@ -2328,7 +2420,7 @@
       <c r="D114" s="15"/>
       <c r="E114" s="15"/>
       <c r="F114" s="15"/>
-      <c r="G114" s="21"/>
+      <c r="G114" s="26"/>
       <c r="H114" s="17"/>
       <c r="I114" s="17"/>
       <c r="J114" s="17"/>
@@ -2342,7 +2434,7 @@
       <c r="D115" s="15"/>
       <c r="E115" s="15"/>
       <c r="F115" s="15"/>
-      <c r="G115" s="21"/>
+      <c r="G115" s="26"/>
       <c r="H115" s="17"/>
       <c r="I115" s="17"/>
       <c r="J115" s="17"/>
@@ -2356,7 +2448,7 @@
       <c r="D116" s="15"/>
       <c r="E116" s="15"/>
       <c r="F116" s="15"/>
-      <c r="G116" s="21"/>
+      <c r="G116" s="26"/>
       <c r="H116" s="17"/>
       <c r="I116" s="17"/>
       <c r="J116" s="17"/>
@@ -2370,7 +2462,7 @@
       <c r="D117" s="15"/>
       <c r="E117" s="15"/>
       <c r="F117" s="15"/>
-      <c r="G117" s="21"/>
+      <c r="G117" s="26"/>
       <c r="H117" s="17"/>
       <c r="I117" s="17"/>
       <c r="J117" s="17"/>
@@ -2384,7 +2476,7 @@
       <c r="D118" s="15"/>
       <c r="E118" s="15"/>
       <c r="F118" s="15"/>
-      <c r="G118" s="21"/>
+      <c r="G118" s="26"/>
       <c r="H118" s="17"/>
       <c r="I118" s="17"/>
       <c r="J118" s="17"/>
@@ -2398,7 +2490,7 @@
       <c r="D119" s="15"/>
       <c r="E119" s="15"/>
       <c r="F119" s="15"/>
-      <c r="G119" s="21"/>
+      <c r="G119" s="26"/>
       <c r="H119" s="17"/>
       <c r="I119" s="17"/>
       <c r="J119" s="17"/>
@@ -2412,7 +2504,7 @@
       <c r="D120" s="15"/>
       <c r="E120" s="15"/>
       <c r="F120" s="15"/>
-      <c r="G120" s="21"/>
+      <c r="G120" s="26"/>
       <c r="H120" s="17"/>
       <c r="I120" s="17"/>
       <c r="J120" s="17"/>
@@ -2426,7 +2518,7 @@
       <c r="D121" s="15"/>
       <c r="E121" s="15"/>
       <c r="F121" s="15"/>
-      <c r="G121" s="21"/>
+      <c r="G121" s="26"/>
       <c r="H121" s="17"/>
       <c r="I121" s="17"/>
       <c r="J121" s="17"/>
@@ -2440,7 +2532,7 @@
       <c r="D122" s="15"/>
       <c r="E122" s="15"/>
       <c r="F122" s="15"/>
-      <c r="G122" s="21"/>
+      <c r="G122" s="26"/>
       <c r="H122" s="17"/>
       <c r="I122" s="17"/>
       <c r="J122" s="17"/>

</xml_diff>

<commit_message>
Updated diary for thuc nguyen
</commit_message>
<xml_diff>
--- a/diaries/diary-thuc-nguyen.xlsx
+++ b/diaries/diary-thuc-nguyen.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -267,6 +267,22 @@
   </si>
   <si>
     <t>The activity as a whole wasn't too exhausting. Since I learned how to look through and read code more quickly using IntelliJ, searching for relevant classes and files wasn't difficult. What was difficult was choosing which features were essential to the system, because this system's purpose is solely to provide plugins that users can use when they play Runescape. The entitrety of the plugins made up the system, with each plugin independent of each other and within their own packages. We decided to choose the PluginManager because that class handles all existing as well as new plugins and the IdleNotifierPlugin as a core plugin because it was essential the gameplay.</t>
+  </si>
+  <si>
+    <t>Understand what was mental simulation.
+The next 3 key expert practicies.
+How do we use mental simulation with code</t>
+  </si>
+  <si>
+    <t>1) Learned what mental simulation was
+2) Learned that we use diagrams and concrete values as we step through code
+3) Learned to be skeptical of the code, of others, and of ourselves.</t>
+  </si>
+  <si>
+    <t>I learned that mental simulation was our way of imagining how the code works, and stepping through the code, thinking of the probably results without actually running the program. This was a way for us to tackle being skeptical of our code, since experts usually use print statements or debuggers to make sure that the value of something is actually that value. However, they simulate going through the code without running the program first. It is also helpful to draw diagrams and possible if-else situations, and stepping through it, simulating it. We have to ask ourselves what we are unsure of after every line of code.</t>
+  </si>
+  <si>
+    <t>The activity gave another interesting perspective on how we deal with reading code, especially one within a large system that we have to understand. Like the mental models lecture, I felt that this lecture was also very helpful.</t>
   </si>
   <si>
     <t>&lt;what day?&gt;</t>
@@ -418,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -483,6 +499,12 @@
     </xf>
     <xf borderId="4" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="11" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -1109,26 +1131,24 @@
       <c r="L17" s="17"/>
     </row>
     <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="23">
+        <v>43867.0</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="D18" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="E18" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="F18" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="G18" s="22" t="s">
         <v>70</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" s="23" t="s">
-        <v>73</v>
       </c>
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
@@ -1138,25 +1158,25 @@
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="A19" s="15" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" s="23" t="s">
-        <v>73</v>
+        <v>76</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>77</v>
       </c>
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
@@ -1166,25 +1186,25 @@
     </row>
     <row r="20" ht="14.25" customHeight="1">
       <c r="A20" s="15" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="G20" s="23" t="s">
-        <v>73</v>
+        <v>76</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>77</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
@@ -1194,25 +1214,25 @@
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="15" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" s="23" t="s">
-        <v>73</v>
+        <v>76</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>77</v>
       </c>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>

</xml_diff>

<commit_message>
Updated diary for thuc nguyen (#363)
</commit_message>
<xml_diff>
--- a/diaries/diary-thuc-nguyen.xlsx
+++ b/diaries/diary-thuc-nguyen.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -283,6 +283,40 @@
   </si>
   <si>
     <t>The activity gave another interesting perspective on how we deal with reading code, especially one within a large system that we have to understand. Like the mental models lecture, I felt that this lecture was also very helpful.</t>
+  </si>
+  <si>
+    <t>Review the class survey
+Understand the next key expert practices
+What are stakeholders? The functionality of our system? The key developers?</t>
+  </si>
+  <si>
+    <t>1) Future topics to cover in the class, feedback on the most and least useful topics. 
+2) Key Expert Practices
+    #7. Prioritize among stakeholders
+    #8. Move along levels of abstraction
+    #9. Do something else
+3) Stakeholders, essential functional and essential non-functional aspects of the system, and key developers such as core maintainers, team members, developers, testers, triagers, documentation writers</t>
+  </si>
+  <si>
+    <t>It was interesting to step away from code and look at other aspects of our system, in a higher level view. I felt that we learned how to read code very well from the past lectures, and that we were able to find the core or essence of our system, but not about who made this project, and the people that were interested in its growth.</t>
+  </si>
+  <si>
+    <t>Satisfied, and enlightened to take pm a different perspective about the system.</t>
+  </si>
+  <si>
+    <t>8:00pm - 11:00pm</t>
+  </si>
+  <si>
+    <t>Learn and share our research on the stakeholders, functionality, key developers, and the issues of our system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We found and described the stakeholders, functionality, key developers, and 5 issues that we can potentially solve. </t>
+  </si>
+  <si>
+    <t>It was surprising to find that our system was solely lead by a single developer, Adam. He does have a team of core maintainers however. Our system also had more stakeholders than I had expected, including the people of Venezuela how play the game even today, in order to convert in-game currency to real money because their economy's financial infrastructure is hyperinflated. The way we went about searching for this information was very straightforward. We looked through Github, the Runelite website, Jagex's website, google, and so on.</t>
+  </si>
+  <si>
+    <t>Surprised especially because it was the first time I read that a game and client had an impact on people's livelihoods.</t>
   </si>
   <si>
     <t>&lt;what day?&gt;</t>
@@ -1157,26 +1191,24 @@
       <c r="L18" s="17"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="23">
+        <v>43874.0</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="24"/>
+      <c r="D19" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="E19" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="F19" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="G19" s="22" t="s">
         <v>74</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="G19" s="25" t="s">
-        <v>77</v>
       </c>
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
@@ -1185,26 +1217,26 @@
       <c r="L19" s="17"/>
     </row>
     <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" s="15" t="s">
+      <c r="A20" s="23">
+        <v>43880.0</v>
+      </c>
+      <c r="B20" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="C20" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="G20" s="25" t="s">
+      <c r="E20" s="21" t="s">
         <v>77</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="22" t="s">
+        <v>79</v>
       </c>
       <c r="H20" s="17"/>
       <c r="I20" s="17"/>
@@ -1214,25 +1246,25 @@
     </row>
     <row r="21" ht="14.25" customHeight="1">
       <c r="A21" s="15" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="H21" s="17"/>
       <c r="I21" s="17"/>

</xml_diff>